<commit_message>
feat: updated excel file
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -1,37 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/bitbucket/powin-backend/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Work/Development/SixFeetUp/2023_DjangoConUS_DjangoUnchained/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABAA92-6CEC-2B40-AA39-767D6C61589A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBD266F-DEDC-9A40-85CD-346A737A8BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="34400" windowHeight="28800" xr2:uid="{1610861B-C36E-1B4D-977E-D5C9A958DED7}"/>
+    <workbookView xWindow="25760" yWindow="500" windowWidth="34400" windowHeight="28800" xr2:uid="{1610861B-C36E-1B4D-977E-D5C9A958DED7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="constant_throughput">'[1]Project Details'!$D$18</definedName>
+    <definedName name="constant_throughput">#REF!</definedName>
     <definedName name="ConstantThroughput">Sheet1!$Q$61</definedName>
     <definedName name="Cycles">Sheet1!$Q$59</definedName>
-    <definedName name="ProjECap">'[1]Project Details'!$D$14</definedName>
+    <definedName name="ProjECap">#REF!</definedName>
     <definedName name="ProjectECap">Sheet1!$Q$62</definedName>
     <definedName name="ProjectElosses">Sheet1!$Q$64</definedName>
     <definedName name="ProjectMinECapacity">Sheet1!$Q$63</definedName>
-    <definedName name="ProjELosses">'[1]Project Details'!$D$28</definedName>
-    <definedName name="ProjMinECapacity">'[1]Project Details'!$D$19</definedName>
-    <definedName name="StackType">'[1]Project Details'!$D$37</definedName>
+    <definedName name="ProjELosses">#REF!</definedName>
+    <definedName name="ProjMinECapacity">#REF!</definedName>
+    <definedName name="StackType">#REF!</definedName>
     <definedName name="Term">Sheet1!$Q$60</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -174,18 +171,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="12">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;?_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.0000000000"/>
-    <numFmt numFmtId="168" formatCode="0.000%"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00000_);\(#,##0.00000\)"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000000_);\(#,##0.000000\)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;?_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00000000_);\(#,##0.00000000\)"/>
-    <numFmt numFmtId="176" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;?_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="0.0000000000"/>
+    <numFmt numFmtId="170" formatCode="0.000%"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00000_);\(#,##0.00000\)"/>
+    <numFmt numFmtId="172" formatCode="#,##0.000000_);\(#,##0.000000\)"/>
+    <numFmt numFmtId="173" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;?_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="#,##0.00000000_);\(#,##0.00000000\)"/>
+    <numFmt numFmtId="175" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -525,10 +522,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -536,7 +533,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -557,59 +554,59 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="174" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -617,16 +614,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -636,8 +633,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="5" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -645,18 +642,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -707,268 +701,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Input"/>
-      <sheetName val="Project Details"/>
-      <sheetName val="Augmentation"/>
-      <sheetName val="PG Tables"/>
-      <sheetName val="RTE"/>
-      <sheetName val="Aux"/>
-      <sheetName val="Project Details Export"/>
-      <sheetName val="PCS Spec"/>
-      <sheetName val="Product Spec"/>
-      <sheetName val="REV Notes"/>
-      <sheetName val="Rev Test"/>
-      <sheetName val="Pricing Output"/>
-      <sheetName val="Summary"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="14">
-          <cell r="D14">
-            <v>400</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18" t="str">
-            <v>Yes</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19">
-            <v>400</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="D28">
-            <v>6.4969673223039703E-2</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="D37" t="str">
-            <v>S750 4+ hrs</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="10">
-          <cell r="C10">
-            <v>365</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>730</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>1095</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>1460</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>1825</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>2190</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>2555</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>2920</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>3285</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>3650</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>4015</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>4380</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>4745</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>5110</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>5475</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>5840</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>6205</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>6570</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>6935</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>7300</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>7665</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>8030</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>8395</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>8760</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>9125</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>9490</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>9855</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>10220</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>10585</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>10950</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>11315</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>11680</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>12045</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43">
-            <v>12410</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="C44">
-            <v>12775</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>13140</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="C46">
-            <v>13505</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47">
-            <v>13870</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48">
-            <v>14235</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1270,7 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9BC61BF-9C93-2148-A7AE-3699F9A1134A}">
   <dimension ref="B50:CL181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H32" zoomScaleNormal="56" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="56" workbookViewId="0">
       <selection activeCell="P67" sqref="P67"/>
     </sheetView>
   </sheetViews>
@@ -1542,7 +1274,6 @@
         <v>2</v>
       </c>
       <c r="D53" s="9">
-        <f>[1]Augmentation!C10</f>
         <v>365</v>
       </c>
       <c r="E53" s="18">
@@ -1552,11 +1283,11 @@
         <v>0.85531416006610039</v>
       </c>
       <c r="G53" s="12">
-        <f>IF(OR(C53&gt;(Cycles+1), F53=0),G52,IF(Term="no",D53*ConstantThroughput*AVERAGE(F53,F52),D53*ProjectMinECapacity))</f>
+        <f t="shared" ref="G53:G91" si="1">IF(OR(C53&gt;(Cycles+1), F53=0),G52,IF(Term="no",D53*ConstantThroughput*AVERAGE(F53,F52),D53*ProjectMinECapacity))</f>
         <v>146000</v>
       </c>
       <c r="H53" s="19">
-        <f>+G53/(1-ProjectElosses)</f>
+        <f t="shared" ref="H53:H91" si="2">+G53/(1-ProjectElosses)</f>
         <v>156149.73262032084</v>
       </c>
       <c r="I53" s="20">
@@ -1639,7 +1370,6 @@
         <v>3</v>
       </c>
       <c r="D54" s="9">
-        <f>[1]Augmentation!C11</f>
         <v>730</v>
       </c>
       <c r="E54" s="18">
@@ -1649,19 +1379,19 @@
         <v>0.82630402805275438</v>
       </c>
       <c r="G54" s="12">
-        <f>IF(OR(C54&gt;(Cycles+1), F54=0),G53,IF(Term="no",D54*ConstantThroughput*AVERAGE(F54,F53),D54*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>292000</v>
       </c>
       <c r="H54" s="19">
-        <f>+G54/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>312299.46524064167</v>
       </c>
       <c r="I54" s="20">
-        <f t="shared" ref="I54:I91" si="1">IF((+H54-H53)&lt;0, 0, +H54-H53)</f>
+        <f t="shared" ref="I54:I91" si="3">IF((+H54-H53)&lt;0, 0, +H54-H53)</f>
         <v>156149.73262032084</v>
       </c>
       <c r="J54" s="21">
-        <f t="shared" ref="J54:J91" si="2">IFERROR(I54/T98,0)</f>
+        <f t="shared" ref="J54:J91" si="4">IFERROR(I54/T98,0)</f>
         <v>345.93418165741457</v>
       </c>
       <c r="K54" s="22">
@@ -1746,7 +1476,6 @@
         <v>4</v>
       </c>
       <c r="D55" s="9">
-        <f>[1]Augmentation!C12</f>
         <v>1095</v>
       </c>
       <c r="E55" s="18">
@@ -1756,19 +1485,19 @@
         <v>0.81482159817066291</v>
       </c>
       <c r="G55" s="12">
-        <f>IF(OR(C55&gt;(Cycles+1), F55=0),G54,IF(Term="no",D55*ConstantThroughput*AVERAGE(F55,F54),D55*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>438000</v>
       </c>
       <c r="H55" s="19">
-        <f>+G55/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>468449.19786096254</v>
       </c>
       <c r="I55" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032086</v>
       </c>
       <c r="J55" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>356.88506395030578</v>
       </c>
       <c r="K55" s="22">
@@ -1876,7 +1605,6 @@
         <v>5</v>
       </c>
       <c r="D56" s="9">
-        <f>[1]Augmentation!C13</f>
         <v>1460</v>
       </c>
       <c r="E56" s="18">
@@ -1886,19 +1614,19 @@
         <v>0.80534484759449398</v>
       </c>
       <c r="G56" s="12">
-        <f>IF(OR(C56&gt;(Cycles+1), F56=0),G55,IF(Term="no",D56*ConstantThroughput*AVERAGE(F56,F55),D56*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>584000</v>
       </c>
       <c r="H56" s="19">
-        <f>+G56/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>624598.93048128334</v>
       </c>
       <c r="I56" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032081</v>
       </c>
       <c r="J56" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>328.68273494776003</v>
       </c>
       <c r="K56" s="22">
@@ -2016,7 +1744,6 @@
         <v>6</v>
       </c>
       <c r="D57" s="9">
-        <f>[1]Augmentation!C14</f>
         <v>1825</v>
       </c>
       <c r="E57" s="18">
@@ -2026,19 +1753,19 @@
         <v>0.79203027790672964</v>
       </c>
       <c r="G57" s="12">
-        <f>IF(OR(C57&gt;(Cycles+1), F57=0),G56,IF(Term="no",D57*ConstantThroughput*AVERAGE(F57,F56),D57*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>730000</v>
       </c>
       <c r="H57" s="19">
-        <f>+G57/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>780748.66310160421</v>
       </c>
       <c r="I57" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032086</v>
       </c>
       <c r="J57" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>331.84316935684001</v>
       </c>
       <c r="K57" s="22">
@@ -2164,7 +1891,6 @@
         <v>7</v>
       </c>
       <c r="D58" s="9">
-        <f>[1]Augmentation!C15</f>
         <v>2190</v>
       </c>
       <c r="E58" s="18">
@@ -2174,19 +1900,19 @@
         <v>0.78037398981568407</v>
       </c>
       <c r="G58" s="12">
-        <f>IF(OR(C58&gt;(Cycles+1), F58=0),G57,IF(Term="no",D58*ConstantThroughput*AVERAGE(F58,F57),D58*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>876000</v>
       </c>
       <c r="H58" s="19">
-        <f>+G58/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>936898.39572192507</v>
       </c>
       <c r="I58" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032086</v>
       </c>
       <c r="J58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>336.38757955908437</v>
       </c>
       <c r="K58" s="22">
@@ -2320,7 +2046,6 @@
         <v>8</v>
       </c>
       <c r="D59" s="9">
-        <f>[1]Augmentation!C16</f>
         <v>2555</v>
       </c>
       <c r="E59" s="18">
@@ -2330,19 +2055,19 @@
         <v>0.76956732183487842</v>
       </c>
       <c r="G59" s="12">
-        <f>IF(OR(C59&gt;(Cycles+1), F59=0),G58,IF(Term="no",D59*ConstantThroughput*AVERAGE(F59,F58),D59*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>1022000</v>
       </c>
       <c r="H59" s="19">
-        <f>+G59/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>1093048.1283422459</v>
       </c>
       <c r="I59" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032086</v>
       </c>
       <c r="J59" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>340.46941874394918</v>
       </c>
       <c r="K59" s="22">
@@ -2359,7 +2084,7 @@
       <c r="P59" t="s">
         <v>31</v>
       </c>
-      <c r="Q59" s="53">
+      <c r="Q59" s="52">
         <v>365</v>
       </c>
       <c r="T59" s="49">
@@ -2492,7 +2217,6 @@
         <v>9</v>
       </c>
       <c r="D60" s="9">
-        <f>[1]Augmentation!C17</f>
         <v>2920</v>
       </c>
       <c r="E60" s="18">
@@ -2502,19 +2226,19 @@
         <v>0.75954138057759424</v>
       </c>
       <c r="G60" s="12">
-        <f>IF(OR(C60&gt;(Cycles+1), F60=0),G59,IF(Term="no",D60*ConstantThroughput*AVERAGE(F60,F59),D60*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>1168000</v>
       </c>
       <c r="H60" s="19">
-        <f>+G60/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>1249197.8609625667</v>
       </c>
       <c r="I60" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032075</v>
       </c>
       <c r="J60" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>344.34323511157351</v>
       </c>
       <c r="K60" s="22">
@@ -2531,7 +2255,7 @@
       <c r="P60" t="s">
         <v>32</v>
       </c>
-      <c r="Q60" s="53">
+      <c r="Q60" s="52">
         <v>20</v>
       </c>
       <c r="T60" s="49">
@@ -2672,7 +2396,6 @@
         <v>10</v>
       </c>
       <c r="D61" s="9">
-        <f>[1]Augmentation!C18</f>
         <v>3285</v>
       </c>
       <c r="E61" s="18">
@@ -2682,19 +2405,19 @@
         <v>0.74522855994932091</v>
       </c>
       <c r="G61" s="12">
-        <f>IF(OR(C61&gt;(Cycles+1), F61=0),G60,IF(Term="no",D61*ConstantThroughput*AVERAGE(F61,F60),D61*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>1314000</v>
       </c>
       <c r="H61" s="19">
-        <f>+G61/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>1405347.5935828877</v>
       </c>
       <c r="I61" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032098</v>
       </c>
       <c r="J61" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>348.01685780447355</v>
       </c>
       <c r="K61" s="22">
@@ -2711,7 +2434,7 @@
       <c r="P61" t="s">
         <v>33</v>
       </c>
-      <c r="Q61" s="53" t="s">
+      <c r="Q61" s="52" t="s">
         <v>34</v>
       </c>
       <c r="T61" s="49">
@@ -2862,7 +2585,6 @@
         <v>11</v>
       </c>
       <c r="D62" s="9">
-        <f>[1]Augmentation!C19</f>
         <v>3650</v>
       </c>
       <c r="E62" s="18">
@@ -2872,19 +2594,19 @@
         <v>0.73378514557308794</v>
       </c>
       <c r="G62" s="12">
-        <f>IF(OR(C62&gt;(Cycles+1), F62=0),G61,IF(Term="no",D62*ConstantThroughput*AVERAGE(F62,F61),D62*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>1460000</v>
       </c>
       <c r="H62" s="19">
-        <f>+G62/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>1561497.3262032084</v>
       </c>
       <c r="I62" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032075</v>
       </c>
       <c r="J62" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>353.39916631140352</v>
       </c>
       <c r="K62" s="22">
@@ -2901,7 +2623,7 @@
       <c r="P62" t="s">
         <v>35</v>
       </c>
-      <c r="Q62" s="53">
+      <c r="Q62" s="52">
         <v>400</v>
       </c>
       <c r="T62" s="49">
@@ -3060,7 +2782,6 @@
         <v>12</v>
       </c>
       <c r="D63" s="9">
-        <f>[1]Augmentation!C20</f>
         <v>4015</v>
       </c>
       <c r="E63" s="18">
@@ -3070,19 +2791,19 @@
         <v>0.7200790878947767</v>
       </c>
       <c r="G63" s="12">
-        <f>IF(OR(C63&gt;(Cycles+1), F63=0),G62,IF(Term="no",D63*ConstantThroughput*AVERAGE(F63,F62),D63*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>1606000</v>
       </c>
       <c r="H63" s="19">
-        <f>+G63/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>1717647.0588235294</v>
       </c>
       <c r="I63" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032098</v>
       </c>
       <c r="J63" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>357.82370306932444</v>
       </c>
       <c r="K63" s="22">
@@ -3099,7 +2820,7 @@
       <c r="P63" t="s">
         <v>36</v>
       </c>
-      <c r="Q63" s="53">
+      <c r="Q63" s="52">
         <v>400</v>
       </c>
       <c r="T63" s="49">
@@ -3266,7 +2987,6 @@
         <v>13</v>
       </c>
       <c r="D64" s="9">
-        <f>[1]Augmentation!C21</f>
         <v>4380</v>
       </c>
       <c r="E64" s="18">
@@ -3276,19 +2996,19 @@
         <v>0.70676332687182331</v>
       </c>
       <c r="G64" s="12">
-        <f>IF(OR(C64&gt;(Cycles+1), F64=0),G63,IF(Term="no",D64*ConstantThroughput*AVERAGE(F64,F63),D64*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>1752000</v>
       </c>
       <c r="H64" s="19">
-        <f>+G64/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>1873796.7914438501</v>
       </c>
       <c r="I64" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032075</v>
       </c>
       <c r="J64" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>330.21844263768463</v>
       </c>
       <c r="K64" s="22">
@@ -3305,7 +3025,7 @@
       <c r="P64" t="s">
         <v>37</v>
       </c>
-      <c r="Q64" s="53">
+      <c r="Q64" s="52">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="T64" s="49">
@@ -3470,7 +3190,6 @@
         <v>14</v>
       </c>
       <c r="D65" s="9">
-        <f>[1]Augmentation!C22</f>
         <v>4745</v>
       </c>
       <c r="E65" s="18">
@@ -3480,19 +3199,19 @@
         <v>0.69532065487482309</v>
       </c>
       <c r="G65" s="12">
-        <f>IF(OR(C65&gt;(Cycles+1), F65=0),G64,IF(Term="no",D65*ConstantThroughput*AVERAGE(F65,F64),D65*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>1898000</v>
       </c>
       <c r="H65" s="19">
-        <f>+G65/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>2029946.5240641709</v>
       </c>
       <c r="I65" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032075</v>
       </c>
       <c r="J65" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>334.71856869586304</v>
       </c>
       <c r="K65" s="22">
@@ -3662,7 +3381,6 @@
         <v>15</v>
       </c>
       <c r="D66" s="9">
-        <f>[1]Augmentation!C23</f>
         <v>5110</v>
       </c>
       <c r="E66" s="18">
@@ -3672,19 +3390,19 @@
         <v>0.68367693834810928</v>
       </c>
       <c r="G66" s="12">
-        <f>IF(OR(C66&gt;(Cycles+1), F66=0),G65,IF(Term="no",D66*ConstantThroughput*AVERAGE(F66,F65),D66*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2044000</v>
       </c>
       <c r="H66" s="19">
-        <f>+G66/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>2186096.2566844919</v>
       </c>
       <c r="I66" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032098</v>
       </c>
       <c r="J66" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>338.68482291376426</v>
       </c>
       <c r="K66" s="22">
@@ -3846,7 +3564,6 @@
         <v>16</v>
       </c>
       <c r="D67" s="9">
-        <f>[1]Augmentation!C24</f>
         <v>5475</v>
       </c>
       <c r="E67" s="18">
@@ -3856,19 +3573,19 @@
         <v>0.67164038063352072</v>
       </c>
       <c r="G67" s="12">
-        <f>IF(OR(C67&gt;(Cycles+1), F67=0),G66,IF(Term="no",D67*ConstantThroughput*AVERAGE(F67,F66),D67*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2190000</v>
       </c>
       <c r="H67" s="19">
-        <f>+G67/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>2342245.9893048126</v>
       </c>
       <c r="I67" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032075</v>
       </c>
       <c r="J67" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>342.81842888662754</v>
       </c>
       <c r="K67" s="22">
@@ -4022,7 +3739,6 @@
         <v>17</v>
       </c>
       <c r="D68" s="9">
-        <f>[1]Augmentation!C25</f>
         <v>5840</v>
       </c>
       <c r="E68" s="18">
@@ -4032,19 +3748,19 @@
         <v>0.65763604864309877</v>
       </c>
       <c r="G68" s="12">
-        <f>IF(OR(C68&gt;(Cycles+1), F68=0),G67,IF(Term="no",D68*ConstantThroughput*AVERAGE(F68,F67),D68*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2336000</v>
       </c>
       <c r="H68" s="19">
-        <f>+G68/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>2498395.7219251334</v>
       </c>
       <c r="I68" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032075</v>
       </c>
       <c r="J68" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>347.19891572327003</v>
       </c>
       <c r="K68" s="22">
@@ -4192,7 +3908,6 @@
         <v>18</v>
       </c>
       <c r="D69" s="9">
-        <f>[1]Augmentation!C26</f>
         <v>6205</v>
       </c>
       <c r="E69" s="18">
@@ -4202,19 +3917,19 @@
         <v>0.64598301526466395</v>
       </c>
       <c r="G69" s="12">
-        <f>IF(OR(C69&gt;(Cycles+1), F69=0),G68,IF(Term="no",D69*ConstantThroughput*AVERAGE(F69,F68),D69*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2482000</v>
       </c>
       <c r="H69" s="19">
-        <f>+G69/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>2654545.4545454546</v>
       </c>
       <c r="I69" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032121</v>
       </c>
       <c r="J69" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>352.43855913301496</v>
       </c>
       <c r="K69" s="22">
@@ -4354,7 +4069,6 @@
         <v>19</v>
       </c>
       <c r="D70" s="9">
-        <f>[1]Augmentation!C27</f>
         <v>6570</v>
       </c>
       <c r="E70" s="18">
@@ -4364,19 +4078,19 @@
         <v>0.63532679770221367</v>
       </c>
       <c r="G70" s="12">
-        <f>IF(OR(C70&gt;(Cycles+1), F70=0),G69,IF(Term="no",D70*ConstantThroughput*AVERAGE(F70,F69),D70*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2628000</v>
       </c>
       <c r="H70" s="19">
-        <f>+G70/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>2810695.1871657753</v>
       </c>
       <c r="I70" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032075</v>
       </c>
       <c r="J70" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>356.92055575187345</v>
       </c>
       <c r="K70" s="22">
@@ -4510,7 +4224,6 @@
         <v>20</v>
       </c>
       <c r="D71" s="9">
-        <f>[1]Augmentation!C28</f>
         <v>6935</v>
       </c>
       <c r="E71" s="18">
@@ -4520,19 +4233,19 @@
         <v>0.62650380545409334</v>
       </c>
       <c r="G71" s="12">
-        <f>IF(OR(C71&gt;(Cycles+1), F71=0),G70,IF(Term="no",D71*ConstantThroughput*AVERAGE(F71,F70),D71*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2774000</v>
       </c>
       <c r="H71" s="19">
-        <f>+G71/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>2966844.9197860961</v>
       </c>
       <c r="I71" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032075</v>
       </c>
       <c r="J71" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>361.12011659534295</v>
       </c>
       <c r="K71" s="22">
@@ -4660,7 +4373,6 @@
         <v>21</v>
       </c>
       <c r="D72" s="9">
-        <f>[1]Augmentation!C29</f>
         <v>7300</v>
       </c>
       <c r="E72" s="18">
@@ -4670,19 +4382,19 @@
         <v>0.6176821620191395</v>
       </c>
       <c r="G72" s="12">
-        <f>IF(OR(C72&gt;(Cycles+1), F72=0),G71,IF(Term="no",D72*ConstantThroughput*AVERAGE(F72,F71),D72*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H72" s="19">
-        <f>+G72/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I72" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156149.73262032075</v>
       </c>
       <c r="J72" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>364.67273391780014</v>
       </c>
       <c r="K72" s="22">
@@ -4794,7 +4506,6 @@
         <v>22</v>
       </c>
       <c r="D73" s="9">
-        <f>[1]Augmentation!C30</f>
         <v>7665</v>
       </c>
       <c r="E73" s="18">
@@ -4804,19 +4515,19 @@
         <v>0</v>
       </c>
       <c r="G73" s="12">
-        <f>IF(OR(C73&gt;(Cycles+1), F73=0),G72,IF(Term="no",D73*ConstantThroughput*AVERAGE(F73,F72),D73*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H73" s="19">
-        <f>+G73/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I73" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J73" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K73" s="22">
@@ -4908,7 +4619,6 @@
         <v>23</v>
       </c>
       <c r="D74" s="9">
-        <f>[1]Augmentation!C31</f>
         <v>8030</v>
       </c>
       <c r="E74" s="18">
@@ -4918,19 +4628,19 @@
         <v>0</v>
       </c>
       <c r="G74" s="12">
-        <f>IF(OR(C74&gt;(Cycles+1), F74=0),G73,IF(Term="no",D74*ConstantThroughput*AVERAGE(F74,F73),D74*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H74" s="19">
-        <f>+G74/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I74" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J74" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K74" s="22">
@@ -4965,7 +4675,6 @@
         <v>24</v>
       </c>
       <c r="D75" s="9">
-        <f>[1]Augmentation!C32</f>
         <v>8395</v>
       </c>
       <c r="E75" s="18">
@@ -4975,19 +4684,19 @@
         <v>0</v>
       </c>
       <c r="G75" s="12">
-        <f>IF(OR(C75&gt;(Cycles+1), F75=0),G74,IF(Term="no",D75*ConstantThroughput*AVERAGE(F75,F74),D75*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H75" s="19">
-        <f>+G75/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I75" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J75" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K75" s="22">
@@ -5028,7 +4737,6 @@
         <v>25</v>
       </c>
       <c r="D76" s="9">
-        <f>[1]Augmentation!C33</f>
         <v>8760</v>
       </c>
       <c r="E76" s="18">
@@ -5038,19 +4746,19 @@
         <v>0</v>
       </c>
       <c r="G76" s="12">
-        <f>IF(OR(C76&gt;(Cycles+1), F76=0),G75,IF(Term="no",D76*ConstantThroughput*AVERAGE(F76,F75),D76*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H76" s="19">
-        <f>+G76/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I76" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J76" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K76" s="22">
@@ -5206,7 +4914,6 @@
         <v>26</v>
       </c>
       <c r="D77" s="9">
-        <f>[1]Augmentation!C34</f>
         <v>9125</v>
       </c>
       <c r="E77" s="18">
@@ -5216,19 +4923,19 @@
         <v>0</v>
       </c>
       <c r="G77" s="12">
-        <f>IF(OR(C77&gt;(Cycles+1), F77=0),G76,IF(Term="no",D77*ConstantThroughput*AVERAGE(F77,F76),D77*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H77" s="19">
-        <f>+G77/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I77" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J77" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K77" s="22">
@@ -5308,7 +5015,6 @@
         <v>27</v>
       </c>
       <c r="D78" s="9">
-        <f>[1]Augmentation!C35</f>
         <v>9490</v>
       </c>
       <c r="E78" s="18">
@@ -5318,19 +5024,19 @@
         <v>0</v>
       </c>
       <c r="G78" s="12">
-        <f>IF(OR(C78&gt;(Cycles+1), F78=0),G77,IF(Term="no",D78*ConstantThroughput*AVERAGE(F78,F77),D78*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H78" s="19">
-        <f>+G78/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I78" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J78" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K78" s="22">
@@ -5420,7 +5126,6 @@
         <v>28</v>
       </c>
       <c r="D79" s="9">
-        <f>[1]Augmentation!C36</f>
         <v>9855</v>
       </c>
       <c r="E79" s="18">
@@ -5430,19 +5135,19 @@
         <v>0</v>
       </c>
       <c r="G79" s="12">
-        <f>IF(OR(C79&gt;(Cycles+1), F79=0),G78,IF(Term="no",D79*ConstantThroughput*AVERAGE(F79,F78),D79*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H79" s="19">
-        <f>+G79/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I79" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J79" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K79" s="22">
@@ -5540,7 +5245,6 @@
         <v>29</v>
       </c>
       <c r="D80" s="9">
-        <f>[1]Augmentation!C37</f>
         <v>10220</v>
       </c>
       <c r="E80" s="18">
@@ -5550,19 +5254,19 @@
         <v>0</v>
       </c>
       <c r="G80" s="12">
-        <f>IF(OR(C80&gt;(Cycles+1), F80=0),G79,IF(Term="no",D80*ConstantThroughput*AVERAGE(F80,F79),D80*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H80" s="19">
-        <f>+G80/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I80" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J80" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K80" s="22">
@@ -5670,7 +5374,6 @@
         <v>30</v>
       </c>
       <c r="D81" s="9">
-        <f>[1]Augmentation!C38</f>
         <v>10585</v>
       </c>
       <c r="E81" s="18">
@@ -5680,19 +5383,19 @@
         <v>0</v>
       </c>
       <c r="G81" s="12">
-        <f>IF(OR(C81&gt;(Cycles+1), F81=0),G80,IF(Term="no",D81*ConstantThroughput*AVERAGE(F81,F80),D81*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H81" s="19">
-        <f>+G81/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I81" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J81" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K81" s="22">
@@ -5808,7 +5511,6 @@
         <v>31</v>
       </c>
       <c r="D82" s="9">
-        <f>[1]Augmentation!C39</f>
         <v>10950</v>
       </c>
       <c r="E82" s="18">
@@ -5818,19 +5520,19 @@
         <v>0</v>
       </c>
       <c r="G82" s="12">
-        <f>IF(OR(C82&gt;(Cycles+1), F82=0),G81,IF(Term="no",D82*ConstantThroughput*AVERAGE(F82,F81),D82*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H82" s="19">
-        <f>+G82/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I82" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J82" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K82" s="22">
@@ -5954,7 +5656,6 @@
         <v>32</v>
       </c>
       <c r="D83" s="9">
-        <f>[1]Augmentation!C40</f>
         <v>11315</v>
       </c>
       <c r="E83" s="18">
@@ -5964,19 +5665,19 @@
         <v>0</v>
       </c>
       <c r="G83" s="12">
-        <f>IF(OR(C83&gt;(Cycles+1), F83=0),G82,IF(Term="no",D83*ConstantThroughput*AVERAGE(F83,F82),D83*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H83" s="19">
-        <f>+G83/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I83" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J83" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K83" s="22">
@@ -6110,7 +5811,6 @@
         <v>33</v>
       </c>
       <c r="D84" s="9">
-        <f>[1]Augmentation!C41</f>
         <v>11680</v>
       </c>
       <c r="E84" s="18">
@@ -6120,19 +5820,19 @@
         <v>0</v>
       </c>
       <c r="G84" s="12">
-        <f>IF(OR(C84&gt;(Cycles+1), F84=0),G83,IF(Term="no",D84*ConstantThroughput*AVERAGE(F84,F83),D84*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H84" s="19">
-        <f>+G84/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I84" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J84" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K84" s="22">
@@ -6274,7 +5974,6 @@
         <v>34</v>
       </c>
       <c r="D85" s="9">
-        <f>[1]Augmentation!C42</f>
         <v>12045</v>
       </c>
       <c r="E85" s="18">
@@ -6284,19 +5983,19 @@
         <v>0</v>
       </c>
       <c r="G85" s="12">
-        <f>IF(OR(C85&gt;(Cycles+1), F85=0),G84,IF(Term="no",D85*ConstantThroughput*AVERAGE(F85,F84),D85*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H85" s="19">
-        <f>+G85/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I85" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J85" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K85" s="22">
@@ -6448,7 +6147,6 @@
         <v>35</v>
       </c>
       <c r="D86" s="9">
-        <f>[1]Augmentation!C43</f>
         <v>12410</v>
       </c>
       <c r="E86" s="18">
@@ -6458,19 +6156,19 @@
         <v>0</v>
       </c>
       <c r="G86" s="12">
-        <f>IF(OR(C86&gt;(Cycles+1), F86=0),G85,IF(Term="no",D86*ConstantThroughput*AVERAGE(F86,F85),D86*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H86" s="19">
-        <f>+G86/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I86" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J86" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K86" s="22">
@@ -6626,7 +6324,6 @@
         <v>36</v>
       </c>
       <c r="D87" s="9">
-        <f>[1]Augmentation!C44</f>
         <v>12775</v>
       </c>
       <c r="E87" s="18">
@@ -6636,19 +6333,19 @@
         <v>0</v>
       </c>
       <c r="G87" s="12">
-        <f>IF(OR(C87&gt;(Cycles+1), F87=0),G86,IF(Term="no",D87*ConstantThroughput*AVERAGE(F87,F86),D87*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H87" s="19">
-        <f>+G87/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I87" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J87" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K87" s="22">
@@ -6802,7 +6499,6 @@
         <v>37</v>
       </c>
       <c r="D88" s="9">
-        <f>[1]Augmentation!C45</f>
         <v>13140</v>
       </c>
       <c r="E88" s="18">
@@ -6812,19 +6508,19 @@
         <v>0</v>
       </c>
       <c r="G88" s="12">
-        <f>IF(OR(C88&gt;(Cycles+1), F88=0),G87,IF(Term="no",D88*ConstantThroughput*AVERAGE(F88,F87),D88*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H88" s="19">
-        <f>+G88/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I88" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J88" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K88" s="22">
@@ -6976,7 +6672,6 @@
         <v>38</v>
       </c>
       <c r="D89" s="9">
-        <f>[1]Augmentation!C46</f>
         <v>13505</v>
       </c>
       <c r="E89" s="18">
@@ -6986,19 +6681,19 @@
         <v>0</v>
       </c>
       <c r="G89" s="12">
-        <f>IF(OR(C89&gt;(Cycles+1), F89=0),G88,IF(Term="no",D89*ConstantThroughput*AVERAGE(F89,F88),D89*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H89" s="19">
-        <f>+G89/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I89" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J89" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K89" s="22">
@@ -7150,7 +6845,6 @@
         <v>39</v>
       </c>
       <c r="D90" s="9">
-        <f>[1]Augmentation!C47</f>
         <v>13870</v>
       </c>
       <c r="E90" s="18">
@@ -7160,19 +6854,19 @@
         <v>0</v>
       </c>
       <c r="G90" s="12">
-        <f>IF(OR(C90&gt;(Cycles+1), F90=0),G89,IF(Term="no",D90*ConstantThroughput*AVERAGE(F90,F89),D90*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H90" s="19">
-        <f>+G90/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I90" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J90" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K90" s="22">
@@ -7322,7 +7016,6 @@
         <v>40</v>
       </c>
       <c r="D91" s="9">
-        <f>[1]Augmentation!C48</f>
         <v>14235</v>
       </c>
       <c r="E91" s="18">
@@ -7332,19 +7025,19 @@
         <v>0</v>
       </c>
       <c r="G91" s="12">
-        <f>IF(OR(C91&gt;(Cycles+1), F91=0),G90,IF(Term="no",D91*ConstantThroughput*AVERAGE(F91,F90),D91*ProjectMinECapacity))</f>
+        <f t="shared" si="1"/>
         <v>2920000</v>
       </c>
       <c r="H91" s="19">
-        <f>+G91/(1-ProjectElosses)</f>
+        <f t="shared" si="2"/>
         <v>3122994.6524064168</v>
       </c>
       <c r="I91" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J91" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K91" s="22">
@@ -8175,13 +7868,13 @@
         <f>ABS(L97-G97)</f>
         <v>0</v>
       </c>
-      <c r="T97" s="52">
+      <c r="T97" s="51">
         <v>439.02528735632188</v>
       </c>
-      <c r="U97" s="53">
+      <c r="U97" s="52">
         <v>439.02528735632188</v>
       </c>
-      <c r="V97" s="53">
+      <c r="V97" s="52">
         <v>0</v>
       </c>
       <c r="AN97" s="42">
@@ -8292,7 +7985,7 @@
         <v>2</v>
       </c>
       <c r="E98" s="8">
-        <f t="shared" ref="E98:E136" si="3">D98</f>
+        <f t="shared" ref="E98:E136" si="5">D98</f>
         <v>2</v>
       </c>
       <c r="F98" s="18">
@@ -8321,16 +8014,16 @@
         <v>0.92966719029852007</v>
       </c>
       <c r="M98" s="17">
-        <f t="shared" ref="M98:M117" si="4">ABS(L98-G98)</f>
+        <f t="shared" ref="M98:M108" si="6">ABS(L98-G98)</f>
         <v>4.8695877336391025E-4</v>
       </c>
-      <c r="T98" s="54">
+      <c r="T98" s="53">
         <v>451.38567074287846</v>
       </c>
-      <c r="U98" s="53">
+      <c r="U98" s="52">
         <v>408.3611925819589</v>
       </c>
-      <c r="V98" s="53">
+      <c r="V98" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8339,7 +8032,7 @@
         <v>3</v>
       </c>
       <c r="E99" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="F99" s="18">
@@ -8357,7 +8050,7 @@
         <v>297415.82759680669</v>
       </c>
       <c r="J99" s="21">
-        <f t="shared" ref="J99:J136" si="5">IF(H99&gt;0, H99/U98, 0)</f>
+        <f t="shared" ref="J99:J136" si="7">IF(H99&gt;0, H99/U98, 0)</f>
         <v>345.93418165741457</v>
       </c>
       <c r="K99" s="32">
@@ -8368,17 +8061,17 @@
         <v>0.897915415844595</v>
       </c>
       <c r="M99" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.9021466277530141E-4</v>
       </c>
       <c r="O99" s="50"/>
-      <c r="T99" s="54">
+      <c r="T99" s="53">
         <v>437.5350733144266</v>
       </c>
-      <c r="U99" s="53">
+      <c r="U99" s="52">
         <v>394.51059515350704</v>
       </c>
-      <c r="V99" s="53">
+      <c r="V99" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8387,7 +8080,7 @@
         <v>4</v>
       </c>
       <c r="E100" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="F100" s="18">
@@ -8397,7 +8090,7 @@
         <v>0.88611848801059578</v>
       </c>
       <c r="H100" s="28">
-        <f t="shared" ref="H100:H136" si="6">IF(E100&lt;2, 0, IFERROR(I55*(U99/T99),0))</f>
+        <f t="shared" ref="H100:H136" si="8">IF(E100&lt;2, 0, IFERROR(I55*(U99/T99),0))</f>
         <v>140794.93898043258</v>
       </c>
       <c r="I100" s="31">
@@ -8405,7 +8098,7 @@
         <v>438210.76657723926</v>
       </c>
       <c r="J100" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>356.88506395030583</v>
       </c>
       <c r="K100" s="32">
@@ -8416,16 +8109,16 @@
         <v>0.88401241278525722</v>
       </c>
       <c r="M100" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.1060752253385662E-3</v>
       </c>
-      <c r="T100" s="54">
+      <c r="T100" s="53">
         <v>475.07738015244041</v>
       </c>
-      <c r="U100" s="53">
+      <c r="U100" s="52">
         <v>389.0284238306013</v>
       </c>
-      <c r="V100" s="53">
+      <c r="V100" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8434,7 +8127,7 @@
         <v>5</v>
       </c>
       <c r="E101" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="F101" s="18">
@@ -8444,7 +8137,7 @@
         <v>0.87581252175901236</v>
       </c>
       <c r="H101" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>127866.92631705839</v>
       </c>
       <c r="I101" s="31">
@@ -8452,7 +8145,7 @@
         <v>566077.69289429765</v>
       </c>
       <c r="J101" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>328.68273494776003</v>
       </c>
       <c r="K101" s="32">
@@ -8463,16 +8156,16 @@
         <v>0.87280689324076233</v>
       </c>
       <c r="M101" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.0056285182500364E-3</v>
       </c>
-      <c r="T101" s="54">
+      <c r="T101" s="53">
         <v>470.55280035735439</v>
       </c>
-      <c r="U101" s="53">
+      <c r="U101" s="52">
         <v>384.50384403551527</v>
       </c>
-      <c r="V101" s="53">
+      <c r="V101" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8481,7 +8174,7 @@
         <v>6</v>
       </c>
       <c r="E102" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="F102" s="18">
@@ -8491,7 +8184,7 @@
         <v>0.86133292722356847</v>
       </c>
       <c r="H102" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>127594.97423463348</v>
       </c>
       <c r="I102" s="31">
@@ -8499,7 +8192,7 @@
         <v>693672.66712893115</v>
       </c>
       <c r="J102" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>331.84316935684001</v>
       </c>
       <c r="K102" s="32">
@@ -8510,16 +8203,16 @@
         <v>0.85920063096118215</v>
       </c>
       <c r="M102" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.1322962623863129E-3</v>
       </c>
-      <c r="T102" s="54">
+      <c r="T102" s="53">
         <v>464.19589220562807</v>
       </c>
-      <c r="U102" s="53">
+      <c r="U102" s="52">
         <v>378.14693588378896</v>
       </c>
-      <c r="V102" s="53">
+      <c r="V102" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8528,7 +8221,7 @@
         <v>7</v>
       </c>
       <c r="E103" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="F103" s="18">
@@ -8538,7 +8231,7 @@
         <v>0.84865671392455633</v>
       </c>
       <c r="H103" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>127203.93247963203</v>
       </c>
       <c r="I103" s="31">
@@ -8546,7 +8239,7 @@
         <v>820876.59960856312</v>
       </c>
       <c r="J103" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>336.38757955908437</v>
       </c>
       <c r="K103" s="32">
@@ -8557,16 +8250,16 @@
         <v>0.84698044761531766</v>
       </c>
       <c r="M103" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.676266309238672E-3</v>
       </c>
-      <c r="T103" s="54">
+      <c r="T103" s="53">
         <v>458.63071401943927</v>
       </c>
-      <c r="U103" s="53">
+      <c r="U103" s="52">
         <v>372.58175769760015</v>
       </c>
-      <c r="V103" s="53">
+      <c r="V103" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8575,7 +8268,7 @@
         <v>8</v>
       </c>
       <c r="E104" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="F104" s="18">
@@ -8585,7 +8278,7 @@
         <v>0.83690446249543027</v>
       </c>
       <c r="H104" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>126852.69447790082</v>
       </c>
       <c r="I104" s="31">
@@ -8593,7 +8286,7 @@
         <v>947729.29408646398</v>
       </c>
       <c r="J104" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>340.46941874394912</v>
       </c>
       <c r="K104" s="32">
@@ -8604,16 +8297,16 @@
         <v>0.83569214765801347</v>
       </c>
       <c r="M104" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2123148374167947E-3</v>
       </c>
-      <c r="T104" s="54">
+      <c r="T104" s="53">
         <v>453.47117845868348</v>
       </c>
-      <c r="U104" s="53">
+      <c r="U104" s="52">
         <v>367.42222213684437</v>
       </c>
-      <c r="V104" s="53">
+      <c r="V104" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8622,7 +8315,7 @@
         <v>9</v>
       </c>
       <c r="E105" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="F105" s="18">
@@ -8632,7 +8325,7 @@
         <v>0.82600125137813363</v>
       </c>
       <c r="H105" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>126519.35662248419</v>
       </c>
       <c r="I105" s="31">
@@ -8640,7 +8333,7 @@
         <v>1074248.6507089483</v>
       </c>
       <c r="J105" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>344.34323511157351</v>
       </c>
       <c r="K105" s="32">
@@ -8651,16 +8344,16 @@
         <v>0.82245149056033884</v>
       </c>
       <c r="M105" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.5497608177947892E-3</v>
       </c>
-      <c r="T105" s="54">
+      <c r="T105" s="53">
         <v>448.68439306480565</v>
       </c>
-      <c r="U105" s="53">
+      <c r="U105" s="52">
         <v>362.63543674296653</v>
       </c>
-      <c r="V105" s="53">
+      <c r="V105" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8669,7 +8362,7 @@
         <v>10</v>
       </c>
       <c r="E106" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="F106" s="18">
@@ -8679,7 +8372,7 @@
         <v>0.81043605894488635</v>
       </c>
       <c r="H106" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>126203.24522384015</v>
       </c>
       <c r="I106" s="31">
@@ -8687,7 +8380,7 @@
         <v>1200451.8959327885</v>
       </c>
       <c r="J106" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>348.01685780447355</v>
       </c>
       <c r="K106" s="32">
@@ -8698,16 +8391,16 @@
         <v>0.80647642581607648</v>
       </c>
       <c r="M106" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.9596331288098696E-3</v>
       </c>
-      <c r="T106" s="54">
+      <c r="T106" s="53">
         <v>441.85087998404282</v>
       </c>
-      <c r="U106" s="53">
+      <c r="U106" s="52">
         <v>355.80192366220371</v>
       </c>
-      <c r="V106" s="53">
+      <c r="V106" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8716,7 +8409,7 @@
         <v>11</v>
       </c>
       <c r="E107" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="F107" s="18">
@@ -8726,7 +8419,7 @@
         <v>0.79799134581073305</v>
       </c>
       <c r="H107" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>125740.10319421643</v>
       </c>
       <c r="I107" s="31">
@@ -8734,7 +8427,7 @@
         <v>1326191.999127005</v>
       </c>
       <c r="J107" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>353.39916631140352</v>
       </c>
       <c r="K107" s="32">
@@ -8745,16 +8438,16 @@
         <v>0.79432122634202595</v>
       </c>
       <c r="M107" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.6701194687071004E-3</v>
       </c>
-      <c r="T107" s="54">
+      <c r="T107" s="53">
         <v>436.38733622425423</v>
       </c>
-      <c r="U107" s="53">
+      <c r="U107" s="52">
         <v>350.33837990241511</v>
       </c>
-      <c r="V107" s="53">
+      <c r="V107" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8763,7 +8456,7 @@
         <v>12</v>
       </c>
       <c r="E108" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="F108" s="18">
@@ -8773,7 +8466,7 @@
         <v>0.78308600808556961</v>
       </c>
       <c r="H108" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>125359.37642398996</v>
       </c>
       <c r="I108" s="31">
@@ -8781,7 +8474,7 @@
         <v>1451551.3755509949</v>
       </c>
       <c r="J108" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>357.82370306932444</v>
       </c>
       <c r="K108" s="32">
@@ -8792,16 +8485,16 @@
         <v>0.77836119207894494</v>
       </c>
       <c r="M108" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.7248160066246658E-3</v>
       </c>
-      <c r="T108" s="54">
+      <c r="T108" s="53">
         <v>472.86799420724083</v>
       </c>
-      <c r="U108" s="53">
+      <c r="U108" s="52">
         <v>343.79455972448216</v>
       </c>
-      <c r="V108" s="53">
+      <c r="V108" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8810,7 +8503,7 @@
         <v>13</v>
       </c>
       <c r="E109" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="F109" s="18">
@@ -8820,7 +8513,7 @@
         <v>0.76860511797310782</v>
       </c>
       <c r="H109" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>113527.30409952697</v>
       </c>
       <c r="I109" s="31">
@@ -8828,7 +8521,7 @@
         <v>1565078.6796505218</v>
       </c>
       <c r="J109" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>330.21844263768469</v>
       </c>
       <c r="K109" s="32">
@@ -8842,13 +8535,13 @@
         <f>ABS(L109-G109)</f>
         <v>6.3672731565389551E-3</v>
       </c>
-      <c r="T109" s="54">
+      <c r="T109" s="53">
         <v>466.51051726444206</v>
       </c>
-      <c r="U109" s="53">
+      <c r="U109" s="52">
         <v>337.43708278168339</v>
       </c>
-      <c r="V109" s="53">
+      <c r="V109" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8857,7 +8550,7 @@
         <v>14</v>
       </c>
       <c r="E110" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="F110" s="18">
@@ -8867,7 +8560,7 @@
         <v>0.75616121217637011</v>
       </c>
       <c r="H110" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>112946.45737359252</v>
       </c>
       <c r="I110" s="31">
@@ -8875,7 +8568,7 @@
         <v>1678025.1370241144</v>
       </c>
       <c r="J110" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>334.71856869586304</v>
       </c>
       <c r="K110" s="32">
@@ -8886,16 +8579,16 @@
         <v>0.74965120635287885</v>
       </c>
       <c r="M110" s="17">
-        <f t="shared" ref="M110:M129" si="7">ABS(L110-G110)</f>
+        <f t="shared" ref="M110:M128" si="9">ABS(L110-G110)</f>
         <v>6.5100058234912606E-3</v>
       </c>
-      <c r="T110" s="54">
+      <c r="T110" s="53">
         <v>461.04732794619417</v>
       </c>
-      <c r="U110" s="53">
+      <c r="U110" s="52">
         <v>331.9738934634355</v>
       </c>
-      <c r="V110" s="53">
+      <c r="V110" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8904,7 +8597,7 @@
         <v>15</v>
       </c>
       <c r="E111" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="F111" s="18">
@@ -8914,7 +8607,7 @@
         <v>0.74349867045356877</v>
       </c>
       <c r="H111" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>112434.51931965651</v>
       </c>
       <c r="I111" s="31">
@@ -8922,7 +8615,7 @@
         <v>1790459.6563437709</v>
       </c>
       <c r="J111" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>338.68482291376432</v>
       </c>
       <c r="K111" s="32">
@@ -8933,16 +8626,16 @@
         <v>0.73869124330115365</v>
       </c>
       <c r="M111" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4.8074271524151113E-3</v>
       </c>
-      <c r="T111" s="54">
+      <c r="T111" s="53">
         <v>455.48815192767995</v>
       </c>
-      <c r="U111" s="53">
+      <c r="U111" s="52">
         <v>326.41471744492128</v>
       </c>
-      <c r="V111" s="53">
+      <c r="V111" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8951,7 +8644,7 @@
         <v>16</v>
       </c>
       <c r="E112" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="F112" s="18">
@@ -8961,7 +8654,7 @@
         <v>0.73040891393895369</v>
       </c>
       <c r="H112" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>111900.98059994038</v>
       </c>
       <c r="I112" s="31">
@@ -8969,7 +8662,7 @@
         <v>1902360.6369437112</v>
       </c>
       <c r="J112" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>342.81842888662754</v>
       </c>
       <c r="K112" s="32">
@@ -8980,16 +8673,16 @@
         <v>0.72673583558937827</v>
       </c>
       <c r="M112" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.6730783495754205E-3</v>
       </c>
-      <c r="T112" s="54">
+      <c r="T112" s="53">
         <v>449.74141781242679</v>
       </c>
-      <c r="U112" s="53">
+      <c r="U112" s="52">
         <v>320.66798332966812</v>
       </c>
-      <c r="V112" s="53">
+      <c r="V112" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -8998,7 +8691,7 @@
         <v>17</v>
       </c>
       <c r="E113" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="F113" s="18">
@@ -9008,7 +8701,7 @@
         <v>0.71517920289936976</v>
       </c>
       <c r="H113" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>111335.57611922841</v>
       </c>
       <c r="I113" s="31">
@@ -9016,7 +8709,7 @@
         <v>2013696.2130629397</v>
       </c>
       <c r="J113" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>347.19891572327009</v>
       </c>
       <c r="K113" s="32">
@@ -9027,16 +8720,16 @@
         <v>0.71178525528660541</v>
       </c>
       <c r="M113" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.3939476127643475E-3</v>
       </c>
-      <c r="T113" s="54">
+      <c r="T113" s="53">
         <v>443.05518954691968</v>
       </c>
-      <c r="U113" s="53">
+      <c r="U113" s="52">
         <v>313.98175506416101</v>
       </c>
-      <c r="V113" s="53">
+      <c r="V113" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9045,7 +8738,7 @@
         <v>18</v>
       </c>
       <c r="E114" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="F114" s="18">
@@ -9055,7 +8748,7 @@
         <v>0.70250652910032196</v>
       </c>
       <c r="H114" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>110659.27734886814</v>
       </c>
       <c r="I114" s="31">
@@ -9063,7 +8756,7 @@
         <v>2124355.4904118078</v>
       </c>
       <c r="J114" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>352.43855913301502</v>
       </c>
       <c r="K114" s="32">
@@ -9074,16 +8767,16 @@
         <v>0.69883957255272799</v>
       </c>
       <c r="M114" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.6669565475939692E-3</v>
       </c>
-      <c r="T114" s="54">
+      <c r="T114" s="53">
         <v>437.49156529071979</v>
       </c>
-      <c r="U114" s="53">
+      <c r="U114" s="52">
         <v>308.41813080796112</v>
       </c>
-      <c r="V114" s="53">
+      <c r="V114" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9092,7 +8785,7 @@
         <v>19</v>
       </c>
       <c r="E115" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="F115" s="18">
@@ -9102,7 +8795,7 @@
         <v>0.69091789250115732</v>
       </c>
       <c r="H115" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>110080.7706519315</v>
       </c>
       <c r="I115" s="31">
@@ -9110,7 +8803,7 @@
         <v>2234436.2610637392</v>
       </c>
       <c r="J115" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>356.92055575187351</v>
       </c>
       <c r="K115" s="32">
@@ -9121,16 +8814,16 @@
         <v>0.68689511791880076</v>
       </c>
       <c r="M115" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4.0227745823565586E-3</v>
       </c>
-      <c r="T115" s="54">
+      <c r="T115" s="53">
         <v>432.40386077770358</v>
       </c>
-      <c r="U115" s="53">
+      <c r="U115" s="52">
         <v>303.33042629494491</v>
       </c>
-      <c r="V115" s="53">
+      <c r="V115" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9139,7 +8832,7 @@
         <v>20</v>
       </c>
       <c r="E116" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="F116" s="18">
@@ -9149,7 +8842,7 @@
         <v>0.68132288843132649</v>
       </c>
       <c r="H116" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>109538.71891054558</v>
       </c>
       <c r="I116" s="31">
@@ -9157,7 +8850,7 @@
         <v>2343974.9799742848</v>
       </c>
       <c r="J116" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>361.12011659534289</v>
       </c>
       <c r="K116" s="32">
@@ -9168,16 +8861,16 @@
         <v>0.67695987913694156</v>
       </c>
       <c r="M116" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4.3630092943849341E-3</v>
       </c>
-      <c r="T116" s="54">
+      <c r="T116" s="53">
         <v>428.191411358761</v>
       </c>
-      <c r="U116" s="53">
+      <c r="U116" s="52">
         <v>299.11797687600233</v>
       </c>
-      <c r="V116" s="53">
+      <c r="V116" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9186,7 +8879,7 @@
         <v>21</v>
       </c>
       <c r="E117" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="F117" s="18">
@@ -9196,7 +8889,7 @@
         <v>0.67172935119581412</v>
       </c>
       <c r="H117" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>109080.17039133309</v>
       </c>
       <c r="I117" s="31">
@@ -9204,7 +8897,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J117" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>364.67273391780009</v>
       </c>
       <c r="K117" s="32">
@@ -9215,16 +8908,16 @@
         <v>0.66702855543061734</v>
       </c>
       <c r="M117" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4.7007957651967747E-3</v>
       </c>
-      <c r="T117" s="54">
+      <c r="T117" s="53">
         <v>423.97960591717663</v>
       </c>
-      <c r="U117" s="53">
+      <c r="U117" s="52">
         <v>294.90617143441796</v>
       </c>
-      <c r="V117" s="53">
+      <c r="V117" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9233,7 +8926,7 @@
         <v>22</v>
       </c>
       <c r="E118" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="F118" s="18">
@@ -9243,7 +8936,7 @@
         <v>0</v>
       </c>
       <c r="H118" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I118" s="31">
@@ -9251,7 +8944,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J118" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K118" s="32">
@@ -9262,16 +8955,16 @@
         <v>0</v>
       </c>
       <c r="M118" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T118" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T118" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U118" s="53">
-        <v>0</v>
-      </c>
-      <c r="V118" s="53">
+      <c r="U118" s="52">
+        <v>0</v>
+      </c>
+      <c r="V118" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9280,7 +8973,7 @@
         <v>23</v>
       </c>
       <c r="E119" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="F119" s="18">
@@ -9290,7 +8983,7 @@
         <v>0</v>
       </c>
       <c r="H119" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I119" s="31">
@@ -9298,7 +8991,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J119" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K119" s="32">
@@ -9309,16 +9002,16 @@
         <v>0</v>
       </c>
       <c r="M119" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T119" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T119" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U119" s="53">
-        <v>0</v>
-      </c>
-      <c r="V119" s="53">
+      <c r="U119" s="52">
+        <v>0</v>
+      </c>
+      <c r="V119" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9327,7 +9020,7 @@
         <v>24</v>
       </c>
       <c r="E120" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="F120" s="18">
@@ -9337,7 +9030,7 @@
         <v>0</v>
       </c>
       <c r="H120" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I120" s="31">
@@ -9345,7 +9038,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J120" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K120" s="32">
@@ -9356,16 +9049,16 @@
         <v>0</v>
       </c>
       <c r="M120" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T120" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T120" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U120" s="53">
-        <v>0</v>
-      </c>
-      <c r="V120" s="53">
+      <c r="U120" s="52">
+        <v>0</v>
+      </c>
+      <c r="V120" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9374,7 +9067,7 @@
         <v>25</v>
       </c>
       <c r="E121" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="F121" s="18">
@@ -9384,7 +9077,7 @@
         <v>0</v>
       </c>
       <c r="H121" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I121" s="31">
@@ -9392,7 +9085,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J121" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K121" s="32">
@@ -9403,16 +9096,16 @@
         <v>0</v>
       </c>
       <c r="M121" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T121" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T121" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U121" s="53">
-        <v>0</v>
-      </c>
-      <c r="V121" s="53">
+      <c r="U121" s="52">
+        <v>0</v>
+      </c>
+      <c r="V121" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9421,7 +9114,7 @@
         <v>26</v>
       </c>
       <c r="E122" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="F122" s="18">
@@ -9431,7 +9124,7 @@
         <v>0</v>
       </c>
       <c r="H122" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I122" s="31">
@@ -9439,7 +9132,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J122" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K122" s="32">
@@ -9450,16 +9143,16 @@
         <v>0</v>
       </c>
       <c r="M122" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T122" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T122" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U122" s="53">
-        <v>0</v>
-      </c>
-      <c r="V122" s="53">
+      <c r="U122" s="52">
+        <v>0</v>
+      </c>
+      <c r="V122" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9468,7 +9161,7 @@
         <v>27</v>
       </c>
       <c r="E123" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="F123" s="18">
@@ -9478,7 +9171,7 @@
         <v>0</v>
       </c>
       <c r="H123" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I123" s="31">
@@ -9486,7 +9179,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J123" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K123" s="32">
@@ -9497,16 +9190,16 @@
         <v>0</v>
       </c>
       <c r="M123" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T123" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T123" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U123" s="53">
-        <v>0</v>
-      </c>
-      <c r="V123" s="53">
+      <c r="U123" s="52">
+        <v>0</v>
+      </c>
+      <c r="V123" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9515,7 +9208,7 @@
         <v>28</v>
       </c>
       <c r="E124" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="F124" s="18">
@@ -9525,7 +9218,7 @@
         <v>0</v>
       </c>
       <c r="H124" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I124" s="31">
@@ -9533,7 +9226,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J124" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K124" s="32">
@@ -9544,16 +9237,16 @@
         <v>0</v>
       </c>
       <c r="M124" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T124" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T124" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U124" s="53">
-        <v>0</v>
-      </c>
-      <c r="V124" s="53">
+      <c r="U124" s="52">
+        <v>0</v>
+      </c>
+      <c r="V124" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9562,7 +9255,7 @@
         <v>29</v>
       </c>
       <c r="E125" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="F125" s="18">
@@ -9572,7 +9265,7 @@
         <v>0</v>
       </c>
       <c r="H125" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I125" s="31">
@@ -9580,7 +9273,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J125" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K125" s="32">
@@ -9591,16 +9284,16 @@
         <v>0</v>
       </c>
       <c r="M125" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T125" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T125" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U125" s="53">
-        <v>0</v>
-      </c>
-      <c r="V125" s="53">
+      <c r="U125" s="52">
+        <v>0</v>
+      </c>
+      <c r="V125" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9609,7 +9302,7 @@
         <v>30</v>
       </c>
       <c r="E126" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F126" s="18">
@@ -9619,7 +9312,7 @@
         <v>0</v>
       </c>
       <c r="H126" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I126" s="31">
@@ -9627,7 +9320,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J126" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K126" s="32">
@@ -9638,16 +9331,16 @@
         <v>0</v>
       </c>
       <c r="M126" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T126" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T126" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U126" s="53">
-        <v>0</v>
-      </c>
-      <c r="V126" s="53">
+      <c r="U126" s="52">
+        <v>0</v>
+      </c>
+      <c r="V126" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9656,7 +9349,7 @@
         <v>31</v>
       </c>
       <c r="E127" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="F127" s="18">
@@ -9666,7 +9359,7 @@
         <v>0</v>
       </c>
       <c r="H127" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I127" s="31">
@@ -9674,7 +9367,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J127" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K127" s="32">
@@ -9685,16 +9378,16 @@
         <v>0</v>
       </c>
       <c r="M127" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T127" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T127" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U127" s="53">
-        <v>0</v>
-      </c>
-      <c r="V127" s="53">
+      <c r="U127" s="52">
+        <v>0</v>
+      </c>
+      <c r="V127" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9703,7 +9396,7 @@
         <v>32</v>
       </c>
       <c r="E128" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="F128" s="18">
@@ -9713,7 +9406,7 @@
         <v>0</v>
       </c>
       <c r="H128" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I128" s="31">
@@ -9721,7 +9414,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J128" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K128" s="32">
@@ -9732,16 +9425,16 @@
         <v>0</v>
       </c>
       <c r="M128" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T128" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T128" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U128" s="53">
-        <v>0</v>
-      </c>
-      <c r="V128" s="53">
+      <c r="U128" s="52">
+        <v>0</v>
+      </c>
+      <c r="V128" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9750,7 +9443,7 @@
         <v>33</v>
       </c>
       <c r="E129" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="F129" s="18">
@@ -9760,7 +9453,7 @@
         <v>0</v>
       </c>
       <c r="H129" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I129" s="31">
@@ -9768,7 +9461,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J129" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K129" s="32">
@@ -9782,13 +9475,13 @@
         <f>ABS(L129-G129)</f>
         <v>0</v>
       </c>
-      <c r="T129" s="54">
+      <c r="T129" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U129" s="53">
-        <v>0</v>
-      </c>
-      <c r="V129" s="53">
+      <c r="U129" s="52">
+        <v>0</v>
+      </c>
+      <c r="V129" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9797,7 +9490,7 @@
         <v>34</v>
       </c>
       <c r="E130" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="F130" s="18">
@@ -9807,7 +9500,7 @@
         <v>0</v>
       </c>
       <c r="H130" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I130" s="31">
@@ -9815,7 +9508,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J130" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K130" s="32">
@@ -9826,16 +9519,16 @@
         <v>0</v>
       </c>
       <c r="M130" s="17">
-        <f t="shared" ref="M130:M136" si="8">ABS(L130-G130)</f>
-        <v>0</v>
-      </c>
-      <c r="T130" s="54">
+        <f t="shared" ref="M130:M136" si="10">ABS(L130-G130)</f>
+        <v>0</v>
+      </c>
+      <c r="T130" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U130" s="53">
-        <v>0</v>
-      </c>
-      <c r="V130" s="53">
+      <c r="U130" s="52">
+        <v>0</v>
+      </c>
+      <c r="V130" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9844,7 +9537,7 @@
         <v>35</v>
       </c>
       <c r="E131" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="F131" s="18">
@@ -9854,7 +9547,7 @@
         <v>0</v>
       </c>
       <c r="H131" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I131" s="31">
@@ -9862,7 +9555,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J131" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K131" s="32">
@@ -9873,16 +9566,16 @@
         <v>0</v>
       </c>
       <c r="M131" s="17">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T131" s="54">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T131" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U131" s="53">
-        <v>0</v>
-      </c>
-      <c r="V131" s="53">
+      <c r="U131" s="52">
+        <v>0</v>
+      </c>
+      <c r="V131" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9891,7 +9584,7 @@
         <v>36</v>
       </c>
       <c r="E132" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="F132" s="18">
@@ -9901,7 +9594,7 @@
         <v>0</v>
       </c>
       <c r="H132" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I132" s="31">
@@ -9909,7 +9602,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J132" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K132" s="32">
@@ -9920,16 +9613,16 @@
         <v>0</v>
       </c>
       <c r="M132" s="17">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T132" s="54">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T132" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U132" s="53">
-        <v>0</v>
-      </c>
-      <c r="V132" s="53">
+      <c r="U132" s="52">
+        <v>0</v>
+      </c>
+      <c r="V132" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9938,7 +9631,7 @@
         <v>37</v>
       </c>
       <c r="E133" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="F133" s="18">
@@ -9948,7 +9641,7 @@
         <v>0</v>
       </c>
       <c r="H133" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I133" s="31">
@@ -9956,7 +9649,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J133" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K133" s="32">
@@ -9967,16 +9660,16 @@
         <v>0</v>
       </c>
       <c r="M133" s="17">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T133" s="54">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T133" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U133" s="53">
-        <v>0</v>
-      </c>
-      <c r="V133" s="53">
+      <c r="U133" s="52">
+        <v>0</v>
+      </c>
+      <c r="V133" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -9985,7 +9678,7 @@
         <v>38</v>
       </c>
       <c r="E134" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="F134" s="18">
@@ -9995,7 +9688,7 @@
         <v>0</v>
       </c>
       <c r="H134" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I134" s="31">
@@ -10003,7 +9696,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J134" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K134" s="32">
@@ -10014,16 +9707,16 @@
         <v>0</v>
       </c>
       <c r="M134" s="17">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T134" s="54">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T134" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U134" s="53">
-        <v>0</v>
-      </c>
-      <c r="V134" s="53">
+      <c r="U134" s="52">
+        <v>0</v>
+      </c>
+      <c r="V134" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -10032,7 +9725,7 @@
         <v>39</v>
       </c>
       <c r="E135" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="F135" s="18">
@@ -10042,7 +9735,7 @@
         <v>0</v>
       </c>
       <c r="H135" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I135" s="31">
@@ -10050,7 +9743,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J135" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K135" s="32">
@@ -10061,16 +9754,16 @@
         <v>0</v>
       </c>
       <c r="M135" s="17">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T135" s="54">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T135" s="53">
         <v>129.07343448275861</v>
       </c>
-      <c r="U135" s="53">
-        <v>0</v>
-      </c>
-      <c r="V135" s="53">
+      <c r="U135" s="52">
+        <v>0</v>
+      </c>
+      <c r="V135" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
@@ -10079,7 +9772,7 @@
         <v>40</v>
       </c>
       <c r="E136" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="F136" s="18">
@@ -10089,7 +9782,7 @@
         <v>0</v>
       </c>
       <c r="H136" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I136" s="31">
@@ -10097,7 +9790,7 @@
         <v>2453055.1503656181</v>
       </c>
       <c r="J136" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K136" s="32">
@@ -10108,30 +9801,30 @@
         <v>0</v>
       </c>
       <c r="M136" s="17">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T136" s="55">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T136" s="54">
         <v>129.07343448275861</v>
       </c>
-      <c r="U136" s="53">
-        <v>0</v>
-      </c>
-      <c r="V136" s="53">
+      <c r="U136" s="52">
+        <v>0</v>
+      </c>
+      <c r="V136" s="52">
         <v>43.024478160919543</v>
       </c>
     </row>
     <row r="138" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D138" s="51"/>
-      <c r="E138" s="51"/>
-      <c r="F138" s="51"/>
-      <c r="G138" s="51"/>
-      <c r="H138" s="51"/>
-      <c r="I138" s="51"/>
-      <c r="J138" s="51"/>
-      <c r="K138" s="51"/>
-      <c r="L138" s="51"/>
-      <c r="M138" s="51"/>
+      <c r="D138" s="23"/>
+      <c r="E138" s="23"/>
+      <c r="F138" s="23"/>
+      <c r="G138" s="23"/>
+      <c r="H138" s="23"/>
+      <c r="I138" s="23"/>
+      <c r="J138" s="23"/>
+      <c r="K138" s="23"/>
+      <c r="L138" s="23"/>
+      <c r="M138" s="23"/>
     </row>
     <row r="140" spans="4:22" x14ac:dyDescent="0.2">
       <c r="D140" s="1" t="s">
@@ -10245,7 +9938,7 @@
         <v>0.92966719029852007</v>
       </c>
       <c r="M143" s="17">
-        <f t="shared" ref="M143:M181" si="9">ABS(L143-G143)</f>
+        <f t="shared" ref="M143:M181" si="11">ABS(L143-G143)</f>
         <v>7.0332809701479926E-2</v>
       </c>
     </row>
@@ -10263,7 +9956,7 @@
         <v>1</v>
       </c>
       <c r="H144" s="45">
-        <f t="shared" ref="H144:H181" si="10">IF(E144&lt;2, 0, IFERROR(I54*(V98/T98),0))</f>
+        <f t="shared" ref="H144:H181" si="12">IF(E144&lt;2, 0, IFERROR(I54*(V98/T98),0))</f>
         <v>14883.637643835007</v>
       </c>
       <c r="I144" s="13">
@@ -10271,7 +9964,7 @@
         <v>14883.637643835007</v>
       </c>
       <c r="J144" s="21">
-        <f t="shared" ref="J144:J181" si="11">IF(H144&gt;0, H144/V98, 0)</f>
+        <f t="shared" ref="J144:J181" si="13">IF(H144&gt;0, H144/V98, 0)</f>
         <v>345.93418165741457</v>
       </c>
       <c r="K144" s="32">
@@ -10282,7 +9975,7 @@
         <v>0.897915415844595</v>
       </c>
       <c r="M144" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.102084584155405</v>
       </c>
     </row>
@@ -10300,7 +9993,7 @@
         <v>1</v>
       </c>
       <c r="H145" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>15354.793639888305</v>
       </c>
       <c r="I145" s="13">
@@ -10308,7 +10001,7 @@
         <v>30238.431283723312</v>
       </c>
       <c r="J145" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>356.88506395030578</v>
       </c>
       <c r="K145" s="32">
@@ -10319,7 +10012,7 @@
         <v>0.88401241278525722</v>
       </c>
       <c r="M145" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.11598758721474278</v>
       </c>
     </row>
@@ -10337,7 +10030,7 @@
         <v>1</v>
       </c>
       <c r="H146" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14141.403151631208</v>
       </c>
       <c r="I146" s="13">
@@ -10345,7 +10038,7 @@
         <v>44379.834435354518</v>
       </c>
       <c r="J146" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>328.68273494776003</v>
       </c>
       <c r="K146" s="32">
@@ -10356,7 +10049,7 @@
         <v>0.87280689324076233</v>
       </c>
       <c r="M146" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.12719310675923767</v>
       </c>
     </row>
@@ -10374,7 +10067,7 @@
         <v>1</v>
       </c>
       <c r="H147" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14277.379192843688</v>
       </c>
       <c r="I147" s="13">
@@ -10382,7 +10075,7 @@
         <v>58657.213628198209</v>
       </c>
       <c r="J147" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>331.84316935684001</v>
       </c>
       <c r="K147" s="32">
@@ -10393,7 +10086,7 @@
         <v>0.85920063096118215</v>
       </c>
       <c r="M147" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.14079936903881785</v>
       </c>
     </row>
@@ -10411,7 +10104,7 @@
         <v>1</v>
       </c>
       <c r="H148" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14472.900070344411</v>
       </c>
       <c r="I148" s="13">
@@ -10419,7 +10112,7 @@
         <v>73130.113698542613</v>
       </c>
       <c r="J148" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>336.38757955908437</v>
       </c>
       <c r="K148" s="32">
@@ -10430,7 +10123,7 @@
         <v>0.84698044761531766</v>
       </c>
       <c r="M148" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.15301955238468234</v>
       </c>
     </row>
@@ -10448,7 +10141,7 @@
         <v>1</v>
       </c>
       <c r="H149" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14648.519071210012</v>
       </c>
       <c r="I149" s="13">
@@ -10456,7 +10149,7 @@
         <v>87778.632769752629</v>
       </c>
       <c r="J149" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>340.46941874394918</v>
       </c>
       <c r="K149" s="32">
@@ -10467,7 +10160,7 @@
         <v>0.83569214765801347</v>
       </c>
       <c r="M149" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.16430785234198653</v>
       </c>
     </row>
@@ -10485,7 +10178,7 @@
         <v>1</v>
       </c>
       <c r="H150" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14815.187998918278</v>
       </c>
       <c r="I150" s="13">
@@ -10493,7 +10186,7 @@
         <v>102593.82076867091</v>
       </c>
       <c r="J150" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>344.34323511157351</v>
       </c>
       <c r="K150" s="32">
@@ -10504,7 +10197,7 @@
         <v>0.82245149056033884</v>
       </c>
       <c r="M150" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.17754850943966116</v>
       </c>
     </row>
@@ -10522,7 +10215,7 @@
         <v>1</v>
       </c>
       <c r="H151" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14973.243698240412</v>
       </c>
       <c r="I151" s="13">
@@ -10530,7 +10223,7 @@
         <v>117567.06446691132</v>
       </c>
       <c r="J151" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>348.01685780447349</v>
       </c>
       <c r="K151" s="32">
@@ -10541,7 +10234,7 @@
         <v>0.80647642581607648</v>
       </c>
       <c r="M151" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.19352357418392352</v>
       </c>
     </row>
@@ -10559,7 +10252,7 @@
         <v>1</v>
       </c>
       <c r="H152" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>15204.814713052154</v>
       </c>
       <c r="I152" s="13">
@@ -10567,7 +10260,7 @@
         <v>132771.87917996349</v>
       </c>
       <c r="J152" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>353.39916631140352</v>
       </c>
       <c r="K152" s="32">
@@ -10578,7 +10271,7 @@
         <v>0.79432122634202595</v>
       </c>
       <c r="M152" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.20567877365797405</v>
       </c>
     </row>
@@ -10596,7 +10289,7 @@
         <v>1</v>
       </c>
       <c r="H153" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>15395.178098165507</v>
       </c>
       <c r="I153" s="13">
@@ -10604,7 +10297,7 @@
         <v>148167.05727812901</v>
       </c>
       <c r="J153" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>357.82370306932438</v>
       </c>
       <c r="K153" s="32">
@@ -10615,7 +10308,7 @@
         <v>0.77836119207894494</v>
       </c>
       <c r="M153" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.22163880792105506</v>
       </c>
     </row>
@@ -10633,7 +10326,7 @@
         <v>1</v>
       </c>
       <c r="H154" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14207.476173597925</v>
       </c>
       <c r="I154" s="13">
@@ -10641,7 +10334,7 @@
         <v>162374.53345172692</v>
       </c>
       <c r="J154" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>330.21844263768463</v>
       </c>
       <c r="K154" s="32">
@@ -10652,7 +10345,7 @@
         <v>0.76223784481656887</v>
       </c>
       <c r="M154" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.23776215518343113</v>
       </c>
     </row>
@@ -10670,7 +10363,7 @@
         <v>1</v>
       </c>
       <c r="H155" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14401.091748909406</v>
       </c>
       <c r="I155" s="13">
@@ -10678,7 +10371,7 @@
         <v>176775.62520063634</v>
       </c>
       <c r="J155" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>334.71856869586304</v>
       </c>
       <c r="K155" s="32">
@@ -10689,7 +10382,7 @@
         <v>0.74965120635287885</v>
       </c>
       <c r="M155" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.25034879364712115</v>
       </c>
     </row>
@@ -10707,7 +10400,7 @@
         <v>1</v>
       </c>
       <c r="H156" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14571.737766888155</v>
       </c>
       <c r="I156" s="13">
@@ -10715,7 +10408,7 @@
         <v>191347.3629675245</v>
       </c>
       <c r="J156" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>338.68482291376426</v>
       </c>
       <c r="K156" s="32">
@@ -10726,7 +10419,7 @@
         <v>0.73869124330115365</v>
       </c>
       <c r="M156" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.26130875669884635</v>
       </c>
     </row>
@@ -10744,7 +10437,7 @@
         <v>1</v>
       </c>
       <c r="H157" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14749.584006793455</v>
       </c>
       <c r="I157" s="13">
@@ -10752,7 +10445,7 @@
         <v>206096.94697431795</v>
       </c>
       <c r="J157" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>342.81842888662754</v>
       </c>
       <c r="K157" s="32">
@@ -10763,7 +10456,7 @@
         <v>0.72673583558937827</v>
       </c>
       <c r="M157" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.27326416441062173</v>
       </c>
     </row>
@@ -10781,7 +10474,7 @@
         <v>1</v>
       </c>
       <c r="H158" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14938.052167030777</v>
       </c>
       <c r="I158" s="13">
@@ -10789,7 +10482,7 @@
         <v>221034.99914134873</v>
       </c>
       <c r="J158" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>347.19891572327003</v>
       </c>
       <c r="K158" s="32">
@@ -10800,7 +10493,7 @@
         <v>0.71178525528660541</v>
       </c>
       <c r="M158" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.28821474471339459</v>
       </c>
     </row>
@@ -10818,7 +10511,7 @@
         <v>1</v>
       </c>
       <c r="H159" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>15163.485090484353</v>
       </c>
       <c r="I159" s="13">
@@ -10826,7 +10519,7 @@
         <v>236198.48423183308</v>
       </c>
       <c r="J159" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>352.43855913301496</v>
       </c>
       <c r="K159" s="32">
@@ -10837,7 +10530,7 @@
         <v>0.69883957255272799</v>
       </c>
       <c r="M159" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.30116042744727201</v>
       </c>
     </row>
@@ -10855,7 +10548,7 @@
         <v>1</v>
       </c>
       <c r="H160" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>15356.320656129748</v>
       </c>
       <c r="I160" s="13">
@@ -10863,7 +10556,7 @@
         <v>251554.80488796282</v>
       </c>
       <c r="J160" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>356.92055575187351</v>
       </c>
       <c r="K160" s="32">
@@ -10874,7 +10567,7 @@
         <v>0.68689511791880076</v>
       </c>
       <c r="M160" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.31310488208119924</v>
       </c>
     </row>
@@ -10892,7 +10585,7 @@
         <v>1</v>
       </c>
       <c r="H161" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>15537.00456992505</v>
       </c>
       <c r="I161" s="13">
@@ -10900,7 +10593,7 @@
         <v>267091.8094578879</v>
       </c>
       <c r="J161" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>361.12011659534289</v>
       </c>
       <c r="K161" s="32">
@@ -10911,7 +10604,7 @@
         <v>0.67695987913694156</v>
       </c>
       <c r="M161" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.32304012086305844</v>
       </c>
     </row>
@@ -10929,7 +10622,7 @@
         <v>1</v>
       </c>
       <c r="H162" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>15689.854076329215</v>
       </c>
       <c r="I162" s="13">
@@ -10937,7 +10630,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J162" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>364.67273391780014</v>
       </c>
       <c r="K162" s="32">
@@ -10948,7 +10641,7 @@
         <v>0.66702855543061734</v>
       </c>
       <c r="M162" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.33297144456938266</v>
       </c>
     </row>
@@ -10966,7 +10659,7 @@
         <v>1</v>
       </c>
       <c r="H163" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I163" s="13">
@@ -10974,7 +10667,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J163" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K163" s="32">
@@ -10985,7 +10678,7 @@
         <v>0</v>
       </c>
       <c r="M163" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11003,7 +10696,7 @@
         <v>1</v>
       </c>
       <c r="H164" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I164" s="13">
@@ -11011,7 +10704,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J164" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K164" s="32">
@@ -11022,7 +10715,7 @@
         <v>0</v>
       </c>
       <c r="M164" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11040,7 +10733,7 @@
         <v>1</v>
       </c>
       <c r="H165" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I165" s="13">
@@ -11048,7 +10741,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J165" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K165" s="32">
@@ -11059,7 +10752,7 @@
         <v>0</v>
       </c>
       <c r="M165" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11077,7 +10770,7 @@
         <v>1</v>
       </c>
       <c r="H166" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I166" s="13">
@@ -11085,7 +10778,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J166" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K166" s="32">
@@ -11096,7 +10789,7 @@
         <v>0</v>
       </c>
       <c r="M166" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11114,7 +10807,7 @@
         <v>1</v>
       </c>
       <c r="H167" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I167" s="13">
@@ -11122,7 +10815,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J167" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K167" s="32">
@@ -11133,7 +10826,7 @@
         <v>0</v>
       </c>
       <c r="M167" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11151,7 +10844,7 @@
         <v>1</v>
       </c>
       <c r="H168" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I168" s="13">
@@ -11159,7 +10852,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J168" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K168" s="32">
@@ -11170,7 +10863,7 @@
         <v>0</v>
       </c>
       <c r="M168" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11188,7 +10881,7 @@
         <v>1</v>
       </c>
       <c r="H169" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I169" s="13">
@@ -11196,7 +10889,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J169" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K169" s="32">
@@ -11207,7 +10900,7 @@
         <v>0</v>
       </c>
       <c r="M169" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11225,7 +10918,7 @@
         <v>1</v>
       </c>
       <c r="H170" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I170" s="13">
@@ -11233,7 +10926,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J170" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K170" s="32">
@@ -11244,7 +10937,7 @@
         <v>0</v>
       </c>
       <c r="M170" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11262,7 +10955,7 @@
         <v>1</v>
       </c>
       <c r="H171" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I171" s="13">
@@ -11270,7 +10963,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J171" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K171" s="32">
@@ -11281,7 +10974,7 @@
         <v>0</v>
       </c>
       <c r="M171" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11299,7 +10992,7 @@
         <v>1</v>
       </c>
       <c r="H172" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I172" s="13">
@@ -11307,7 +11000,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J172" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K172" s="32">
@@ -11318,7 +11011,7 @@
         <v>0</v>
       </c>
       <c r="M172" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11336,7 +11029,7 @@
         <v>1</v>
       </c>
       <c r="H173" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I173" s="13">
@@ -11344,7 +11037,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J173" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K173" s="32">
@@ -11355,7 +11048,7 @@
         <v>0</v>
       </c>
       <c r="M173" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11373,7 +11066,7 @@
         <v>1</v>
       </c>
       <c r="H174" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I174" s="13">
@@ -11381,7 +11074,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J174" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K174" s="32">
@@ -11392,7 +11085,7 @@
         <v>0</v>
       </c>
       <c r="M174" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11410,7 +11103,7 @@
         <v>1</v>
       </c>
       <c r="H175" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I175" s="13">
@@ -11418,7 +11111,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J175" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K175" s="32">
@@ -11429,7 +11122,7 @@
         <v>0</v>
       </c>
       <c r="M175" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11447,7 +11140,7 @@
         <v>1</v>
       </c>
       <c r="H176" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I176" s="13">
@@ -11455,7 +11148,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J176" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K176" s="32">
@@ -11466,7 +11159,7 @@
         <v>0</v>
       </c>
       <c r="M176" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11484,7 +11177,7 @@
         <v>1</v>
       </c>
       <c r="H177" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I177" s="13">
@@ -11492,7 +11185,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J177" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K177" s="32">
@@ -11503,7 +11196,7 @@
         <v>0</v>
       </c>
       <c r="M177" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11521,7 +11214,7 @@
         <v>1</v>
       </c>
       <c r="H178" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I178" s="13">
@@ -11529,7 +11222,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J178" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K178" s="32">
@@ -11540,7 +11233,7 @@
         <v>0</v>
       </c>
       <c r="M178" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11558,7 +11251,7 @@
         <v>1</v>
       </c>
       <c r="H179" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I179" s="13">
@@ -11566,7 +11259,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J179" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K179" s="32">
@@ -11577,7 +11270,7 @@
         <v>0</v>
       </c>
       <c r="M179" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11595,7 +11288,7 @@
         <v>1</v>
       </c>
       <c r="H180" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I180" s="13">
@@ -11603,7 +11296,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J180" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K180" s="32">
@@ -11614,7 +11307,7 @@
         <v>0</v>
       </c>
       <c r="M180" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -11632,7 +11325,7 @@
         <v>1</v>
       </c>
       <c r="H181" s="45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I181" s="13">
@@ -11640,7 +11333,7 @@
         <v>282781.66353421711</v>
       </c>
       <c r="J181" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K181" s="32">
@@ -11651,25 +11344,25 @@
         <v>0</v>
       </c>
       <c r="M181" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="M52:M91">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+      <formula>-0.001</formula>
+      <formula>0.001</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M97:M136">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M142:M181">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>-0.001</formula>
-      <formula>0.001</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M52:M91">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>

</xml_diff>